<commit_message>
Transformation of a string to float cell value is applied when it is possible.
</commit_message>
<xml_diff>
--- a/EasyDox.Tests/Invoice.xlsx
+++ b/EasyDox.Tests/Invoice.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slepo\Documents\EasyDox\EasyDox.Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12350" tabRatio="0"/>
+    <workbookView showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760" tabRatio="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,11 +130,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$р.-423]"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -605,7 +600,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -663,9 +658,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -725,6 +717,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -809,14 +804,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,7 +938,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -978,27 +970,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1030,24 +1004,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1223,24 +1179,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AL34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AN23" sqref="AN23"/>
+      <selection activeCell="AJ23" sqref="AJ23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="1.109375" customWidth="1"/>
-    <col min="2" max="38" width="3.44140625" customWidth="1"/>
-    <col min="39" max="39" width="1.109375" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" customWidth="1"/>
+    <col min="2" max="38" width="3.5" customWidth="1"/>
+    <col min="39" max="39" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:38" ht="22.5" customHeight="1" thickBot="1">
       <c r="B1" s="55" t="s">
         <v>13</v>
       </c>
@@ -1281,50 +1237,50 @@
       <c r="AK1" s="55"/>
       <c r="AL1" s="55"/>
     </row>
-    <row r="2" spans="2:38" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+    <row r="2" spans="2:38" ht="12.75">
+      <c r="B2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="40" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="41"/>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="41"/>
-      <c r="Z2" s="41"/>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="41"/>
-      <c r="AH2" s="41"/>
-      <c r="AI2" s="41"/>
-      <c r="AJ2" s="41"/>
-      <c r="AK2" s="41"/>
-      <c r="AL2" s="42"/>
-    </row>
-    <row r="3" spans="2:38" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="40"/>
+      <c r="AK2" s="40"/>
+      <c r="AL2" s="41"/>
+    </row>
+    <row r="3" spans="2:38" ht="12.75">
       <c r="B3" s="64" t="s">
         <v>18</v>
       </c>
@@ -1338,36 +1294,36 @@
       <c r="J3" s="65"/>
       <c r="K3" s="65"/>
       <c r="L3" s="66"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="43" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="45"/>
-    </row>
-    <row r="4" spans="2:38" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="44"/>
+    </row>
+    <row r="4" spans="2:38" ht="12.75">
       <c r="B4" s="64" t="s">
         <v>19</v>
       </c>
@@ -1381,36 +1337,36 @@
       <c r="J4" s="65"/>
       <c r="K4" s="65"/>
       <c r="L4" s="66"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="43" t="s">
+      <c r="M4" s="37"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="44"/>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
-      <c r="AG4" s="44"/>
-      <c r="AH4" s="44"/>
-      <c r="AI4" s="44"/>
-      <c r="AJ4" s="44"/>
-      <c r="AK4" s="44"/>
-      <c r="AL4" s="45"/>
-    </row>
-    <row r="5" spans="2:38" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="44"/>
+    </row>
+    <row r="5" spans="2:38" ht="12.75">
       <c r="B5" s="67" t="s">
         <v>14</v>
       </c>
@@ -1453,7 +1409,7 @@
       <c r="AK5" s="60"/>
       <c r="AL5" s="61"/>
     </row>
-    <row r="6" spans="2:38" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:38" ht="13.5" thickBot="1">
       <c r="B6" s="69" t="s">
         <v>20</v>
       </c>
@@ -1496,7 +1452,7 @@
       <c r="AK6" s="62"/>
       <c r="AL6" s="63"/>
     </row>
-    <row r="7" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:38">
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
@@ -1533,7 +1489,7 @@
       <c r="AK7" s="20"/>
       <c r="AL7" s="20"/>
     </row>
-    <row r="8" spans="2:38" s="17" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:38" s="17" customFormat="1" ht="34.5" customHeight="1" thickBot="1">
       <c r="B8" s="57" t="s">
         <v>33</v>
       </c>
@@ -1574,7 +1530,7 @@
       <c r="AK8" s="57"/>
       <c r="AL8" s="57"/>
     </row>
-    <row r="10" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:38" ht="12.75">
       <c r="B10" s="58" t="s">
         <v>15</v>
       </c>
@@ -1617,12 +1573,12 @@
       <c r="AK10" s="59"/>
       <c r="AL10" s="59"/>
     </row>
-    <row r="11" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:38" ht="12.75">
       <c r="B11" s="1"/>
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="2:38" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:38" ht="13.35" customHeight="1">
       <c r="B12" s="58" t="s">
         <v>16</v>
       </c>
@@ -1665,55 +1621,55 @@
       <c r="AK12" s="59"/>
       <c r="AL12" s="59"/>
     </row>
-    <row r="13" spans="2:38" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:38" ht="13.5" thickBot="1">
       <c r="B13" s="1"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:38" ht="12.75">
       <c r="B14" s="71" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="71"/>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46" t="s">
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
-      <c r="S14" s="46"/>
-      <c r="T14" s="46"/>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="46"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46" t="s">
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="46"/>
-      <c r="AB14" s="46" t="s">
+      <c r="Z14" s="45"/>
+      <c r="AA14" s="45"/>
+      <c r="AB14" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46" t="s">
+      <c r="AC14" s="45"/>
+      <c r="AD14" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AE14" s="46"/>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
+      <c r="AE14" s="45"/>
+      <c r="AF14" s="45"/>
+      <c r="AG14" s="45"/>
       <c r="AH14" s="56" t="s">
         <v>6</v>
       </c>
@@ -1722,7 +1678,7 @@
       <c r="AK14" s="56"/>
       <c r="AL14" s="56"/>
     </row>
-    <row r="15" spans="2:38" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:38" ht="26.25" customHeight="1" thickBot="1">
       <c r="B15" s="50">
         <v>1</v>
       </c>
@@ -1773,7 +1729,7 @@
       <c r="AK15" s="75"/>
       <c r="AL15" s="76"/>
     </row>
-    <row r="16" spans="2:38" ht="6.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:38" ht="6.95" customHeight="1">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1812,7 +1768,7 @@
       <c r="AK16" s="5"/>
       <c r="AL16" s="5"/>
     </row>
-    <row r="17" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:38" ht="12.75">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1831,31 +1787,31 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
-      <c r="T17" s="34" t="s">
+      <c r="T17" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="35"/>
-      <c r="AF17" s="35"/>
-      <c r="AG17" s="35"/>
-      <c r="AH17" s="77" t="s">
+      <c r="U17" s="34"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34"/>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="34"/>
+      <c r="AE17" s="34"/>
+      <c r="AF17" s="34"/>
+      <c r="AG17" s="34"/>
+      <c r="AH17" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AI17" s="77"/>
-      <c r="AJ17" s="77"/>
-      <c r="AK17" s="77"/>
-      <c r="AL17" s="77"/>
-    </row>
-    <row r="18" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+      <c r="AI17" s="46"/>
+      <c r="AJ17" s="46"/>
+      <c r="AK17" s="46"/>
+      <c r="AL17" s="46"/>
+    </row>
+    <row r="18" spans="2:38" ht="12.75">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1890,14 +1846,14 @@
       <c r="AG18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AI18" s="25">
+      <c r="AI18" s="46">
         <v>0</v>
       </c>
-      <c r="AJ18" s="25"/>
-      <c r="AK18" s="25"/>
-      <c r="AL18" s="25"/>
-    </row>
-    <row r="19" spans="2:38" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="AJ18" s="46"/>
+      <c r="AK18" s="46"/>
+      <c r="AL18" s="46"/>
+    </row>
+    <row r="19" spans="2:38" ht="15.75">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1933,14 +1889,14 @@
         <v>24</v>
       </c>
       <c r="AH19" s="22"/>
-      <c r="AI19" s="77" t="s">
+      <c r="AI19" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="AJ19" s="77"/>
-      <c r="AK19" s="77"/>
-      <c r="AL19" s="77"/>
-    </row>
-    <row r="20" spans="2:38" ht="13" x14ac:dyDescent="0.2">
+      <c r="AJ19" s="46"/>
+      <c r="AK19" s="46"/>
+      <c r="AL19" s="46"/>
+    </row>
+    <row r="20" spans="2:38" ht="12.75">
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -1979,8 +1935,8 @@
       <c r="AK20" s="47"/>
       <c r="AL20" s="47"/>
     </row>
-    <row r="21" spans="2:38" ht="6.9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:38" ht="6.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:38" ht="6.95" customHeight="1"/>
+    <row r="22" spans="2:38" ht="6.95" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2019,25 +1975,25 @@
       <c r="AK22" s="5"/>
       <c r="AL22" s="5"/>
     </row>
-    <row r="23" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27" t="s">
+    <row r="23" spans="2:38" ht="26.25" customHeight="1"/>
+    <row r="24" spans="2:38" ht="26.25" customHeight="1">
+      <c r="B24" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
-      <c r="O24" s="28"/>
-      <c r="P24" s="28"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
@@ -2049,64 +2005,64 @@
       <c r="Z24" s="8"/>
       <c r="AA24" s="9"/>
       <c r="AB24" s="10"/>
-      <c r="AC24" s="30" t="s">
+      <c r="AC24" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="AD24" s="30"/>
-      <c r="AE24" s="30"/>
-      <c r="AF24" s="30"/>
-      <c r="AG24" s="30"/>
-      <c r="AH24" s="30"/>
-      <c r="AI24" s="30"/>
-      <c r="AJ24" s="30"/>
-      <c r="AK24" s="30"/>
-      <c r="AL24" s="30"/>
-    </row>
-    <row r="25" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R25" s="26" t="s">
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
+      <c r="AF24" s="29"/>
+      <c r="AG24" s="29"/>
+      <c r="AH24" s="29"/>
+      <c r="AI24" s="29"/>
+      <c r="AJ24" s="29"/>
+      <c r="AK24" s="29"/>
+      <c r="AL24" s="29"/>
+    </row>
+    <row r="25" spans="2:38" ht="26.25" customHeight="1">
+      <c r="R25" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="25"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
+      <c r="AA25" s="25"/>
       <c r="AB25" s="11"/>
-      <c r="AC25" s="26" t="s">
+      <c r="AC25" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AD25" s="26"/>
-      <c r="AE25" s="26"/>
-      <c r="AF25" s="26"/>
-      <c r="AG25" s="26"/>
-      <c r="AH25" s="26"/>
-      <c r="AI25" s="26"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="26"/>
-    </row>
-    <row r="26" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="27" t="s">
+      <c r="AD25" s="25"/>
+      <c r="AE25" s="25"/>
+      <c r="AF25" s="25"/>
+      <c r="AG25" s="25"/>
+      <c r="AH25" s="25"/>
+      <c r="AI25" s="25"/>
+      <c r="AJ25" s="25"/>
+      <c r="AK25" s="25"/>
+      <c r="AL25" s="25"/>
+    </row>
+    <row r="26" spans="2:38" ht="26.25" customHeight="1"/>
+    <row r="27" spans="2:38" ht="26.25" customHeight="1">
+      <c r="B27" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="29"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
@@ -2118,54 +2074,54 @@
       <c r="Z27" s="8"/>
       <c r="AA27" s="9"/>
       <c r="AB27" s="10"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="30"/>
-      <c r="AI27" s="30"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="30"/>
-    </row>
-    <row r="28" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="R28" s="26" t="s">
+      <c r="AC27" s="29"/>
+      <c r="AD27" s="29"/>
+      <c r="AE27" s="29"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+    </row>
+    <row r="28" spans="2:38" ht="26.25" customHeight="1">
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="R28" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="26"/>
-      <c r="Y28" s="26"/>
-      <c r="Z28" s="26"/>
-      <c r="AA28" s="26"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="25"/>
+      <c r="V28" s="25"/>
+      <c r="W28" s="25"/>
+      <c r="X28" s="25"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="25"/>
+      <c r="AA28" s="25"/>
       <c r="AB28" s="11"/>
-      <c r="AC28" s="26" t="s">
+      <c r="AC28" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AD28" s="26"/>
-      <c r="AE28" s="26"/>
-      <c r="AF28" s="26"/>
-      <c r="AG28" s="26"/>
-      <c r="AH28" s="26"/>
-      <c r="AI28" s="26"/>
-      <c r="AJ28" s="26"/>
-      <c r="AK28" s="26"/>
-      <c r="AL28" s="26"/>
-    </row>
-    <row r="29" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD28" s="25"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="25"/>
+      <c r="AG28" s="25"/>
+      <c r="AH28" s="25"/>
+      <c r="AI28" s="25"/>
+      <c r="AJ28" s="25"/>
+      <c r="AK28" s="25"/>
+      <c r="AL28" s="25"/>
+    </row>
+    <row r="29" spans="2:38" ht="26.25" customHeight="1">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -2202,7 +2158,7 @@
       <c r="AK29" s="12"/>
       <c r="AL29" s="12"/>
     </row>
-    <row r="30" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:38" ht="26.25" customHeight="1">
       <c r="B30" s="18" t="s">
         <v>11</v>
       </c>
@@ -2229,50 +2185,50 @@
       <c r="Z30" s="8"/>
       <c r="AA30" s="9"/>
       <c r="AB30" s="10"/>
-      <c r="AC30" s="30"/>
-      <c r="AD30" s="30"/>
-      <c r="AE30" s="30"/>
-      <c r="AF30" s="30"/>
-      <c r="AG30" s="30"/>
-      <c r="AH30" s="30"/>
-      <c r="AI30" s="30"/>
-      <c r="AJ30" s="30"/>
-      <c r="AK30" s="30"/>
-      <c r="AL30" s="30"/>
-    </row>
-    <row r="31" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="R31" s="26" t="s">
+      <c r="AC30" s="29"/>
+      <c r="AD30" s="29"/>
+      <c r="AE30" s="29"/>
+      <c r="AF30" s="29"/>
+      <c r="AG30" s="29"/>
+      <c r="AH30" s="29"/>
+      <c r="AI30" s="29"/>
+      <c r="AJ30" s="29"/>
+      <c r="AK30" s="29"/>
+      <c r="AL30" s="29"/>
+    </row>
+    <row r="31" spans="2:38" ht="26.25" customHeight="1">
+      <c r="R31" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="26"/>
-      <c r="W31" s="26"/>
-      <c r="X31" s="26"/>
-      <c r="Y31" s="26"/>
-      <c r="Z31" s="26"/>
-      <c r="AA31" s="26"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="25"/>
+      <c r="Y31" s="25"/>
+      <c r="Z31" s="25"/>
+      <c r="AA31" s="25"/>
       <c r="AB31" s="11"/>
-      <c r="AC31" s="26" t="s">
+      <c r="AC31" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AD31" s="26"/>
-      <c r="AE31" s="26"/>
-      <c r="AF31" s="26"/>
-      <c r="AG31" s="26"/>
-      <c r="AH31" s="26"/>
-      <c r="AI31" s="26"/>
-      <c r="AJ31" s="26"/>
-      <c r="AK31" s="26"/>
-      <c r="AL31" s="26"/>
-    </row>
-    <row r="32" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="AD31" s="25"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
+      <c r="AH31" s="25"/>
+      <c r="AI31" s="25"/>
+      <c r="AJ31" s="25"/>
+      <c r="AK31" s="25"/>
+      <c r="AL31" s="25"/>
+    </row>
+    <row r="32" spans="2:38" ht="26.25" customHeight="1">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -2306,24 +2262,24 @@
       <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
     </row>
-    <row r="33" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27" t="s">
+    <row r="33" spans="2:38" ht="26.25" customHeight="1">
+      <c r="B33" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
@@ -2335,65 +2291,61 @@
       <c r="Z33" s="8"/>
       <c r="AA33" s="9"/>
       <c r="AB33" s="10"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="30"/>
-      <c r="AE33" s="30"/>
-      <c r="AF33" s="30"/>
-      <c r="AG33" s="30"/>
-      <c r="AH33" s="30"/>
-      <c r="AI33" s="30"/>
-      <c r="AJ33" s="30"/>
-      <c r="AK33" s="30"/>
-      <c r="AL33" s="30"/>
-    </row>
-    <row r="34" spans="2:38" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H34" s="26" t="s">
+      <c r="AC33" s="29"/>
+      <c r="AD33" s="29"/>
+      <c r="AE33" s="29"/>
+      <c r="AF33" s="29"/>
+      <c r="AG33" s="29"/>
+      <c r="AH33" s="29"/>
+      <c r="AI33" s="29"/>
+      <c r="AJ33" s="29"/>
+      <c r="AK33" s="29"/>
+      <c r="AL33" s="29"/>
+    </row>
+    <row r="34" spans="2:38" ht="26.25" customHeight="1">
+      <c r="H34" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-      <c r="R34" s="26" t="s">
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="R34" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
-      <c r="W34" s="26"/>
-      <c r="X34" s="26"/>
-      <c r="Y34" s="26"/>
-      <c r="Z34" s="26"/>
-      <c r="AA34" s="26"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="25"/>
+      <c r="W34" s="25"/>
+      <c r="X34" s="25"/>
+      <c r="Y34" s="25"/>
+      <c r="Z34" s="25"/>
+      <c r="AA34" s="25"/>
       <c r="AB34" s="11"/>
-      <c r="AC34" s="26" t="s">
+      <c r="AC34" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AD34" s="26"/>
-      <c r="AE34" s="26"/>
-      <c r="AF34" s="26"/>
-      <c r="AG34" s="26"/>
-      <c r="AH34" s="26"/>
-      <c r="AI34" s="26"/>
-      <c r="AJ34" s="26"/>
-      <c r="AK34" s="26"/>
-      <c r="AL34" s="26"/>
+      <c r="AD34" s="25"/>
+      <c r="AE34" s="25"/>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="25"/>
+      <c r="AH34" s="25"/>
+      <c r="AI34" s="25"/>
+      <c r="AJ34" s="25"/>
+      <c r="AK34" s="25"/>
+      <c r="AL34" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="H14:X14"/>
-    <mergeCell ref="H12:AL12"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="B4:L4"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="B12:G12"/>
-    <mergeCell ref="H28:P28"/>
-    <mergeCell ref="AC28:AL28"/>
     <mergeCell ref="B1:AL1"/>
     <mergeCell ref="AH14:AL14"/>
     <mergeCell ref="B8:AL8"/>
@@ -2408,12 +2360,16 @@
     <mergeCell ref="B5:L5"/>
     <mergeCell ref="B6:L6"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="H14:X14"/>
+    <mergeCell ref="H12:AL12"/>
     <mergeCell ref="AC24:AL24"/>
     <mergeCell ref="R25:AA25"/>
     <mergeCell ref="AC25:AL25"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="H15:X15"/>
+    <mergeCell ref="AH17:AL17"/>
+    <mergeCell ref="AI19:AL19"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="T17:AG17"/>
     <mergeCell ref="B24:P24"/>
@@ -2430,8 +2386,6 @@
     <mergeCell ref="AB15:AC15"/>
     <mergeCell ref="Y15:AA15"/>
     <mergeCell ref="AD14:AG14"/>
-    <mergeCell ref="AH17:AL17"/>
-    <mergeCell ref="AI19:AL19"/>
     <mergeCell ref="H34:P34"/>
     <mergeCell ref="R34:AA34"/>
     <mergeCell ref="B33:G33"/>
@@ -2446,6 +2400,8 @@
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="H33:P33"/>
     <mergeCell ref="AC33:AL33"/>
+    <mergeCell ref="H28:P28"/>
+    <mergeCell ref="AC28:AL28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>